<commit_message>
Updated docstrings, fixed error in CtoS, added shortcut functions
Updated the documention found in the doc strings for all functions.

Found and corrected an error in how the order of time constants are returned in the C to S function.

Added two helper functions to preset the flags for finding the modulus at time of material functions. Updated the convolution funtions to use these helper functions, to be more readable.
</commit_message>
<xml_diff>
--- a/Data/CtoS_Orig.xlsx
+++ b/Data/CtoS_Orig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\crehb\OneDrive\Research\Undergrad Thesis\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4c98bf736aafef55/Research/Python/Interconversion-Python/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="119" documentId="13_ncr:1_{45CD8B7E-1A80-4211-835F-A9FFC3462F9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2341390B-1CD6-4827-88A0-666E6199BC1D}"/>
+  <xr:revisionPtr revIDLastSave="122" documentId="13_ncr:1_{45CD8B7E-1A80-4211-835F-A9FFC3462F9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9EAF77A8-F28D-4F3C-B830-4C5A31A2D831}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{697B4D84-7E92-469D-B2DC-C89150EC5EC3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{697B4D84-7E92-469D-B2DC-C89150EC5EC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -512,7 +514,7 @@
   <dimension ref="A1:AJ40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:G3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -550,6 +552,9 @@
         <v>368.88</v>
       </c>
     </row>
+    <row r="4" spans="1:36">
+      <c r="C4" s="19"/>
+    </row>
     <row r="5" spans="1:36">
       <c r="A5" t="s">
         <v>0</v>

</xml_diff>